<commit_message>
ran pois, renamed categories to english, saved POI plots to outputs/plots
</commit_message>
<xml_diff>
--- a/input/transport_stats/anzahl_wege_alter15.xlsx
+++ b/input/transport_stats/anzahl_wege_alter15.xlsx
@@ -25,13 +25,13 @@
     <t xml:space="preserve">Altersgruppe</t>
   </si>
   <si>
-    <t xml:space="preserve">Männlich</t>
+    <t xml:space="preserve">männlich</t>
   </si>
   <si>
     <t xml:space="preserve">Ungew. Fallzahl</t>
   </si>
   <si>
-    <t xml:space="preserve">Weiblich</t>
+    <t xml:space="preserve">weiblich</t>
   </si>
   <si>
     <t xml:space="preserve">Alle</t>
@@ -186,10 +186,10 @@
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.14"/>
   </cols>

</xml_diff>